<commit_message>
Dropped index column and added percentage column to each worksheet.
</commit_message>
<xml_diff>
--- a/spreadsheets/Boolean_Analysis_Output.xlsx
+++ b/spreadsheets/Boolean_Analysis_Output.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ljcoo\NSS\Projects\NSS_Capstone_Project\spreadsheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E39E6D7-EC8F-4847-8C59-846F03B83AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="2664" yWindow="3756" windowWidth="17280" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Farmers_Market_EBT" sheetId="1" r:id="rId1"/>
@@ -12,12 +18,22 @@
     <sheet name="FM_Cooking_Demonstrations" sheetId="3" r:id="rId3"/>
     <sheet name="FM_Kids_Activities" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>Accepts EBT</t>
   </si>
@@ -38,13 +54,19 @@
   </si>
   <si>
     <t>Food Activities for Kids</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,6 +76,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -93,20 +122,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -153,7 +196,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -185,9 +228,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -219,6 +280,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -394,41 +473,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="B2">
         <v>131</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C2" s="5">
+        <f>(B2/137)*100</f>
+        <v>95.620437956204384</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="B3">
         <v>6</v>
+      </c>
+      <c r="C3" s="5">
+        <f>(B3/137)*100</f>
+        <v>4.3795620437956204</v>
       </c>
     </row>
   </sheetData>
@@ -437,41 +523,52 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="B2">
         <v>101</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C2" s="5">
+        <f>(B2/138)*100</f>
+        <v>73.188405797101453</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="B3">
         <v>37</v>
+      </c>
+      <c r="C3" s="5">
+        <f>(B3/138)*100</f>
+        <v>26.811594202898554</v>
       </c>
     </row>
   </sheetData>
@@ -480,30 +577,52 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.5546875" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1">
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>138</v>
+      </c>
+      <c r="C2">
+        <f>(B2/138)*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>138</v>
+      <c r="C3">
+        <f>(B3/138)*100</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -512,33 +631,57 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1">
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>138</v>
+      </c>
+      <c r="C2" s="2">
+        <f>(B2/138)*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>138</v>
+      <c r="C3" s="2">
+        <f>(B3/138)*100</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>